<commit_message>
update new user data
</commit_message>
<xml_diff>
--- a/server/data/users.xlsx
+++ b/server/data/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/Nova/lottery/server/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45F853A-DA40-724E-95C1-EDCFDA79E2C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C018E5-6F12-544D-AA9F-ED807337C438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26640" windowHeight="17280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="86">
   <si>
     <t>note</t>
   </si>
@@ -868,7 +868,7 @@
   <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D98" sqref="D98"/>
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.6640625" defaultRowHeight="18"/>
@@ -1708,9 +1708,7 @@
       <c r="B80" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="C80" s="16" t="s">
-        <v>71</v>
-      </c>
+      <c r="C80" s="16"/>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="4"/>

</xml_diff>